<commit_message>
cambios | mejorara repote
</commit_message>
<xml_diff>
--- a/plantillas/FORMATO_BL_CON_FONDO.xlsx
+++ b/plantillas/FORMATO_BL_CON_FONDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\api-backend-general-v1\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33E1F55-4C0B-455F-B759-AFC4EC0B699C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D89840-02EF-4ECB-B50B-8C4EE1B95B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,86 +467,86 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3177,7 +3177,7 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3201,132 +3201,132 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="A4" s="73"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
       <c r="G6" s="2"/>
       <c r="H6" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
       <c r="G7" s="2"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
+      <c r="A9" s="73"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="2"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
     </row>
     <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
+      <c r="A14" s="73"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3343,10 +3343,10 @@
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
       <c r="C17" s="57"/>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="72"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="56"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
@@ -3383,21 +3383,21 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63" t="s">
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
     </row>
     <row r="23" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="29"/>
@@ -3424,27 +3424,27 @@
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="64" t="s">
+      <c r="D26" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
       <c r="G26" s="59"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="60"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
       <c r="G27" s="59"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
       <c r="B28" s="60"/>
       <c r="C28" s="26"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
       <c r="G28" s="59"/>
       <c r="I28" s="2"/>
       <c r="J28" s="20"/>
@@ -3453,18 +3453,18 @@
       <c r="A29" s="60"/>
       <c r="B29" s="60"/>
       <c r="C29" s="23"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
       <c r="G29" s="59"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="60"/>
       <c r="B30" s="60"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
       <c r="G30" s="59"/>
       <c r="I30" s="22"/>
       <c r="J30" s="2"/>
@@ -3473,9 +3473,9 @@
       <c r="A31" s="60"/>
       <c r="B31" s="60"/>
       <c r="C31" s="19"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="59"/>
       <c r="I31" s="9"/>
       <c r="J31" s="10"/>
@@ -3484,9 +3484,9 @@
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
       <c r="C32" s="27"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="59"/>
       <c r="I32" s="25"/>
       <c r="J32" s="11"/>
@@ -3494,9 +3494,9 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
       <c r="G33" s="59"/>
       <c r="I33" s="22"/>
       <c r="J33" s="2"/>
@@ -3513,20 +3513,20 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A35" s="62"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
       <c r="D36" s="26" t="s">
         <v>0</v>
       </c>
@@ -3545,9 +3545,9 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -3566,40 +3566,40 @@
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="67"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
+      <c r="A39" s="71"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="67"/>
+      <c r="A40" s="71"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="71"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="67"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-      <c r="J41" s="67"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
@@ -3661,12 +3661,12 @@
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="68"/>
-      <c r="J50" s="68"/>
+      <c r="E50" s="72"/>
+      <c r="F50" s="72"/>
+      <c r="G50" s="72"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="72"/>
+      <c r="J50" s="72"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
@@ -3712,10 +3712,10 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="66"/>
-      <c r="B57" s="66"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="66"/>
+      <c r="A57" s="70"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="70"/>
       <c r="I57" s="18" t="s">
         <v>0</v>
       </c>
@@ -3728,10 +3728,10 @@
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
-      <c r="B59" s="65"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="65"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="69"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="69"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3749,31 +3749,20 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="65"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="65"/>
-      <c r="H63" s="65"/>
-      <c r="I63" s="65"/>
-      <c r="J63" s="65"/>
+      <c r="A63" s="69"/>
+      <c r="B63" s="69"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+      <c r="H63" s="69"/>
+      <c r="I63" s="69"/>
+      <c r="J63" s="69"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="A63:J63"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A39:J41"/>
-    <mergeCell ref="E50:J50"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A3:E7"/>
@@ -3783,6 +3772,17 @@
     <mergeCell ref="A8:E10"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:G35"/>
+    <mergeCell ref="A63:J63"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A39:J41"/>
+    <mergeCell ref="E50:J50"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
@@ -3841,26 +3841,26 @@
       <c r="K2" s="30"/>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="31"/>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
     </row>
     <row r="4" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="31"/>
       <c r="G4" s="33"/>
       <c r="H4" s="30"/>
@@ -3869,28 +3869,28 @@
       <c r="K4" s="30"/>
     </row>
     <row r="5" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
       <c r="F5" s="31"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
-      <c r="J5" s="83" t="s">
+      <c r="J5" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="83"/>
+      <c r="K5" s="78"/>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="30"/>
@@ -3899,24 +3899,24 @@
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="30"/>
       <c r="I7" s="34"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
       <c r="F8" s="31"/>
       <c r="G8" s="30"/>
       <c r="H8" s="31"/>
@@ -3925,11 +3925,11 @@
       <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
       <c r="F9" s="31"/>
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
@@ -3938,11 +3938,11 @@
       <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="35"/>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
@@ -3951,11 +3951,11 @@
       <c r="K10" s="30"/>
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
       <c r="F11" s="30" t="s">
         <v>0</v>
       </c>
@@ -3966,13 +3966,13 @@
       <c r="K11" s="30"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
       <c r="F12" s="31"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
@@ -3981,11 +3981,11 @@
       <c r="K12" s="30"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
       <c r="F13" s="31"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
@@ -3994,24 +3994,24 @@
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
+      <c r="A14" s="76"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
       <c r="K14" s="30"/>
     </row>
     <row r="15" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
+      <c r="A15" s="76"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
@@ -4023,8 +4023,8 @@
       <c r="A16" s="30"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
       <c r="F16" s="31"/>
       <c r="G16" s="39"/>
       <c r="H16" s="30"/>
@@ -4102,11 +4102,11 @@
       <c r="K21" s="30"/>
     </row>
     <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
-      <c r="B22" s="87"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="40"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
@@ -4115,16 +4115,16 @@
       <c r="K22" s="30"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="79" t="s">
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
       <c r="I23" s="30"/>
@@ -4132,9 +4132,9 @@
       <c r="K23" s="30"/>
     </row>
     <row r="24" spans="1:11" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="75"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="84"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="42"/>
@@ -4147,11 +4147,11 @@
     <row r="25" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
     </row>
     <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -4168,28 +4168,28 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="78" t="s">
+      <c r="E29" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
       <c r="I29" s="30"/>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="63"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="34" t="s">
         <v>11</v>
       </c>
@@ -4199,211 +4199,211 @@
       <c r="K30" s="30"/>
     </row>
     <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="63"/>
-      <c r="B31" s="63"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
       <c r="I31" s="31"/>
       <c r="J31" s="46"/>
       <c r="K31" s="30"/>
     </row>
     <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="63"/>
-      <c r="B32" s="63"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="23"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="85"/>
+      <c r="H32" s="85"/>
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="63"/>
-      <c r="B33" s="63"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="2"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="85"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85"/>
       <c r="I33" s="34"/>
       <c r="J33" s="31"/>
       <c r="K33" s="30"/>
     </row>
     <row r="34" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="63"/>
-      <c r="B34" s="63"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="19"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="47"/>
       <c r="J34" s="48"/>
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="63"/>
-      <c r="B35" s="63"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="27"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
       <c r="I35" s="49"/>
       <c r="J35" s="50"/>
       <c r="K35" s="30"/>
     </row>
     <row r="36" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
+      <c r="A36" s="73"/>
+      <c r="B36" s="73"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="34"/>
       <c r="J36" s="31"/>
       <c r="K36" s="30"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="63"/>
-      <c r="B37" s="63"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="27"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
       <c r="I37" s="31"/>
       <c r="J37" s="31"/>
       <c r="K37" s="30"/>
     </row>
     <row r="38" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="80"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="81"/>
+      <c r="A38" s="86"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="31"/>
       <c r="J38" s="31"/>
       <c r="K38" s="30"/>
     </row>
     <row r="39" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="72"/>
-      <c r="B39" s="72"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="27"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
       <c r="I39" s="34"/>
       <c r="J39" s="31"/>
       <c r="K39" s="30"/>
     </row>
     <row r="40" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="72"/>
-      <c r="B40" s="72"/>
+      <c r="A40" s="64"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="28"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
       <c r="I40" s="51"/>
       <c r="J40" s="51"/>
       <c r="K40" s="30"/>
     </row>
     <row r="41" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="72"/>
-      <c r="B41" s="72"/>
+      <c r="A41" s="64"/>
+      <c r="B41" s="64"/>
       <c r="C41" s="27"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="85"/>
       <c r="I41" s="30"/>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="72"/>
-      <c r="B42" s="72"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="64"/>
       <c r="C42" s="27"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="85"/>
+      <c r="H42" s="85"/>
       <c r="I42" s="43"/>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
     </row>
     <row r="43" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="72"/>
-      <c r="B43" s="72"/>
+      <c r="A43" s="64"/>
+      <c r="B43" s="64"/>
       <c r="C43" s="27"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="78"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
       <c r="I43" s="43"/>
       <c r="J43" s="30"/>
       <c r="K43" s="30"/>
     </row>
     <row r="44" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="72"/>
-      <c r="B44" s="72"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="64"/>
       <c r="C44" s="27"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
       <c r="I44" s="43"/>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
     </row>
     <row r="45" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A45" s="62"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A46" s="75"/>
-      <c r="B46" s="75"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="77"/>
       <c r="H46" s="43"/>
       <c r="I46" s="43"/>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
     </row>
     <row r="47" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="75"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
+      <c r="A47" s="84"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
       <c r="D47" s="30" t="s">
         <v>0</v>
       </c>
@@ -4420,9 +4420,9 @@
       <c r="K47" s="30"/>
     </row>
     <row r="48" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="75"/>
-      <c r="B48" s="75"/>
-      <c r="C48" s="75"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="32"/>
       <c r="E48" s="32"/>
       <c r="F48" s="32"/>
@@ -4446,42 +4446,42 @@
       <c r="K49" s="30"/>
     </row>
     <row r="50" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="77"/>
-      <c r="B50" s="77"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="77"/>
-      <c r="J50" s="77"/>
+      <c r="A50" s="88"/>
+      <c r="B50" s="88"/>
+      <c r="C50" s="88"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="88"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="88"/>
       <c r="K50" s="30"/>
     </row>
     <row r="51" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="77"/>
-      <c r="B51" s="77"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="77"/>
+      <c r="A51" s="88"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="88"/>
+      <c r="E51" s="88"/>
+      <c r="F51" s="88"/>
+      <c r="G51" s="88"/>
+      <c r="H51" s="88"/>
+      <c r="I51" s="88"/>
+      <c r="J51" s="88"/>
       <c r="K51" s="30"/>
     </row>
     <row r="52" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="77"/>
-      <c r="B52" s="77"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="77"/>
-      <c r="E52" s="77"/>
-      <c r="F52" s="77"/>
-      <c r="G52" s="77"/>
-      <c r="H52" s="77"/>
-      <c r="I52" s="77"/>
-      <c r="J52" s="77"/>
+      <c r="A52" s="88"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="88"/>
+      <c r="D52" s="88"/>
+      <c r="E52" s="88"/>
+      <c r="F52" s="88"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
       <c r="K52" s="30"/>
     </row>
     <row r="53" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
@@ -4544,12 +4544,12 @@
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="14"/>
-      <c r="E61" s="68"/>
-      <c r="F61" s="68"/>
-      <c r="G61" s="68"/>
-      <c r="H61" s="68"/>
-      <c r="I61" s="68"/>
-      <c r="J61" s="68"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="72"/>
+      <c r="G61" s="72"/>
+      <c r="H61" s="72"/>
+      <c r="I61" s="72"/>
+      <c r="J61" s="72"/>
     </row>
     <row r="62" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
@@ -4596,10 +4596,10 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="66"/>
-      <c r="B68" s="66"/>
-      <c r="C68" s="66"/>
-      <c r="D68" s="66"/>
+      <c r="A68" s="70"/>
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="70"/>
       <c r="I68" s="18" t="s">
         <v>0</v>
       </c>
@@ -4612,10 +4612,10 @@
       <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
-      <c r="B70" s="65"/>
-      <c r="C70" s="65"/>
-      <c r="D70" s="65"/>
+      <c r="A70" s="69"/>
+      <c r="B70" s="69"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="69"/>
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4633,16 +4633,16 @@
     </row>
     <row r="73" spans="1:10" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="65"/>
-      <c r="B74" s="65"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="65"/>
-      <c r="E74" s="65"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
+      <c r="A74" s="69"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
+      <c r="I74" s="69"/>
+      <c r="J74" s="69"/>
     </row>
     <row r="75" spans="1:10" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:10" ht="13.2" x14ac:dyDescent="0.25"/>
@@ -4658,6 +4658,21 @@
     <row r="86" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A74:J74"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A50:J52"/>
+    <mergeCell ref="E61:J61"/>
+    <mergeCell ref="E29:H44"/>
+    <mergeCell ref="A30:B37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:B44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:G45"/>
     <mergeCell ref="F25:J25"/>
     <mergeCell ref="A3:E5"/>
     <mergeCell ref="F3:G3"/>
@@ -4671,21 +4686,6 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="A23:C24"/>
     <mergeCell ref="D23:F23"/>
-    <mergeCell ref="E29:H44"/>
-    <mergeCell ref="A30:B37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:B44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A74:J74"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A50:J52"/>
-    <mergeCell ref="E61:J61"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="74" orientation="portrait" r:id="rId1"/>

</xml_diff>